<commit_message>
methane work sheet and wetland datafrome
</commit_message>
<xml_diff>
--- a/Methane/Methane_worksheet_Edit.xlsx
+++ b/Methane/Methane_worksheet_Edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Methane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30E457BF-1FD8-0C4C-888B-00BCD629FEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548B3FA7-841E-104F-A08A-A18BEECDC7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="520" windowWidth="25300" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14840" yWindow="1800" windowWidth="33940" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Results and Concentrations" sheetId="2" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
   <si>
     <t>Site</t>
   </si>
@@ -350,6 +350,12 @@
   <si>
     <t>dilution</t>
   </si>
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
 </sst>
 </file>
 
@@ -538,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -719,6 +725,24 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3291,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW815"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3639,7 +3663,7 @@
         <v>2.529265962210544E-3</v>
       </c>
       <c r="Z3" s="22">
-        <f>(((Q3*I3)+((H3*V3*Y3)*10^6))-(U3*I3))/H3</f>
+        <f>(Q3*I3+H3*V3*Y3*10^6-U3*I3)/H3</f>
         <v>146.87999813423636</v>
       </c>
       <c r="AA3" s="22">
@@ -3659,11 +3683,11 @@
         <v>3455.5631519196272</v>
       </c>
       <c r="AE3" s="22">
-        <f t="shared" ref="AE3:AE4" si="0">AD3/AB3*100</f>
+        <f>AD3/AB3*100</f>
         <v>1240.2979576706236</v>
       </c>
       <c r="AF3" s="22">
-        <f t="shared" ref="AF3:AF4" si="1">Z3/AC3*100</f>
+        <f>Z3/AC3*100</f>
         <v>1105.4385143150369</v>
       </c>
       <c r="AG3" s="17">
@@ -3725,7 +3749,7 @@
         <v>0.15100000000000002</v>
       </c>
       <c r="J4" s="14">
-        <f t="shared" ref="J4:J5" si="2">L4*1.7142+83.704</f>
+        <f>L4*1.7142+83.704</f>
         <v>1223.6469999999999</v>
       </c>
       <c r="K4" s="30">
@@ -3795,7 +3819,7 @@
         <v>278.60750157239994</v>
       </c>
       <c r="AC4" s="25">
-        <f t="shared" ref="AC4" si="3">AB4*V4</f>
+        <f>AB4*V4</f>
         <v>12.803548819100774</v>
       </c>
       <c r="AD4" s="25">
@@ -3803,11 +3827,11 @@
         <v>1052.00235193392</v>
       </c>
       <c r="AE4" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AE3:AE4" si="0">AD4/AB4*100</f>
         <v>377.59297434442658</v>
       </c>
       <c r="AF4" s="22">
-        <f t="shared" si="1"/>
+        <f>Z4/AC4*100</f>
         <v>347.84243901208322</v>
       </c>
       <c r="AG4" s="17">
@@ -3869,7 +3893,7 @@
         <v>0.122</v>
       </c>
       <c r="J5" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J4:J5" si="1">L5*1.7142+83.704</f>
         <v>2416.7302</v>
       </c>
       <c r="K5" s="30">
@@ -4002,22 +4026,23 @@
       <c r="L6" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="Q6" s="25" t="s">
+      <c r="Q6" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="S6" s="33" t="s">
+      <c r="R6" s="75"/>
+      <c r="S6" s="76" t="s">
         <v>78</v>
       </c>
       <c r="T6" s="43"/>
@@ -4062,22 +4087,23 @@
       <c r="C7" s="11"/>
       <c r="D7" s="15"/>
       <c r="G7" s="1"/>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="25" t="s">
+      <c r="Q7" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="S7" s="33"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="76"/>
       <c r="T7" s="43"/>
       <c r="U7" s="3"/>
       <c r="W7" s="2"/>
@@ -4106,10 +4132,15 @@
       <c r="C8" s="11"/>
       <c r="D8" s="15"/>
       <c r="G8" s="1"/>
-      <c r="P8" s="23" t="s">
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="33"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="76"/>
       <c r="T8" s="43"/>
       <c r="U8" s="3"/>
       <c r="W8" s="2"/>
@@ -4132,10 +4163,15 @@
       <c r="C9" s="11"/>
       <c r="D9" s="15"/>
       <c r="G9" s="1"/>
-      <c r="P9" s="23" t="s">
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="S9" s="33"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="76"/>
       <c r="T9" s="43"/>
       <c r="U9" s="3"/>
       <c r="W9" s="2"/>
@@ -4151,7 +4187,13 @@
       <c r="C10" s="11"/>
       <c r="D10" s="15"/>
       <c r="G10" s="1"/>
-      <c r="S10" s="33"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="76"/>
       <c r="T10" s="43"/>
       <c r="U10" s="3"/>
       <c r="W10" s="2"/>
@@ -4325,6 +4367,12 @@
       <c r="C20" s="11"/>
       <c r="D20" s="15"/>
       <c r="G20" s="1"/>
+      <c r="O20" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="P20" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="S20" s="33"/>
       <c r="T20" s="43"/>
       <c r="U20" s="3"/>
@@ -4342,6 +4390,14 @@
       <c r="C21" s="11"/>
       <c r="D21" s="15"/>
       <c r="G21" s="1"/>
+      <c r="O21">
+        <f>10^10</f>
+        <v>10000000000</v>
+      </c>
+      <c r="P21" s="23">
+        <f>10^-2.5</f>
+        <v>3.1622776601683764E-3</v>
+      </c>
       <c r="S21" s="33"/>
       <c r="T21" s="43"/>
       <c r="U21" s="3"/>
@@ -4359,6 +4415,14 @@
       <c r="C22" s="11"/>
       <c r="D22" s="15"/>
       <c r="G22" s="1"/>
+      <c r="O22" s="23">
+        <f>10^2.5</f>
+        <v>316.22776601683825</v>
+      </c>
+      <c r="P22">
+        <f>10^0</f>
+        <v>1</v>
+      </c>
       <c r="S22" s="33"/>
       <c r="T22" s="43"/>
       <c r="U22" s="3"/>
@@ -4376,6 +4440,14 @@
       <c r="C23" s="11"/>
       <c r="D23" s="15"/>
       <c r="G23" s="1"/>
+      <c r="O23">
+        <f>10^-5</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P23" s="23">
+        <f>10^2.5</f>
+        <v>316.22776601683825</v>
+      </c>
       <c r="U23" s="3"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>

</xml_diff>